<commit_message>
actualizo data para siniestros 301
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotorTercero.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotorTercero.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB52E564-1791-4D46-B6BB-4DBB74F07E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC360C9-6274-4C4A-B79A-EA165CD3331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="86">
   <si>
     <t>Usuario</t>
   </si>
@@ -646,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AH16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="7" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>6</v>
+        <v>301</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>45</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="8" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>7</v>
+        <v>301</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>45</v>
@@ -1498,419 +1498,835 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
+        <v>301</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P9" s="5">
+        <v>967</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" s="5">
+        <v>25698369</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V9" s="5">
+        <v>2020</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>301</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P10" s="5">
+        <v>967</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S10" s="5">
+        <v>25698369</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="V10" s="5">
+        <v>2020</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH10" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>301</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P11" s="5">
+        <v>967</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11" s="5">
+        <v>25698369</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V11" s="5">
+        <v>2020</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH11" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>301</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P12" s="5">
+        <v>967</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S12" s="5">
+        <v>25698369</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="V12" s="5">
+        <v>2020</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE12" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF12" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH12" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E13" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J13" t="s">
         <v>21</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K13" t="s">
         <v>22</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L13" t="s">
         <v>12</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M13" t="s">
         <v>17</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N13" t="s">
         <v>18</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O13" t="s">
         <v>50</v>
       </c>
-      <c r="P9">
+      <c r="P13">
         <v>967</v>
       </c>
-      <c r="Q9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="Q13" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" t="s">
         <v>23</v>
       </c>
-      <c r="S9">
+      <c r="S13">
         <v>25698369</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T13" t="s">
         <v>53</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U13" t="s">
         <v>57</v>
       </c>
-      <c r="V9">
+      <c r="V13">
         <v>2020</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W13" t="s">
         <v>39</v>
       </c>
-      <c r="X9" t="s">
+      <c r="X13" t="s">
         <v>40</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Y13" t="s">
         <v>41</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="Z13" t="s">
         <v>61</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AA13" t="s">
         <v>31</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AB13" t="s">
         <v>33</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AC13" t="s">
         <v>35</v>
       </c>
-      <c r="AD9" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE9">
-        <v>1</v>
-      </c>
-      <c r="AF9">
-        <v>1</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH9" t="s">
+      <c r="AD13" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE13">
+        <v>1</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E14" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J14" t="s">
         <v>21</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K14" t="s">
         <v>22</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L14" t="s">
         <v>12</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M14" t="s">
         <v>17</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N14" t="s">
         <v>18</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O14" t="s">
         <v>43</v>
       </c>
-      <c r="P10">
+      <c r="P14">
         <v>967</v>
       </c>
-      <c r="Q10" t="s">
-        <v>6</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="Q14" t="s">
+        <v>6</v>
+      </c>
+      <c r="R14" t="s">
         <v>23</v>
       </c>
-      <c r="S10">
+      <c r="S14">
         <v>25698369</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T14" t="s">
         <v>54</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U14" t="s">
         <v>58</v>
       </c>
-      <c r="V10">
+      <c r="V14">
         <v>2020</v>
       </c>
-      <c r="W10" t="s">
+      <c r="W14" t="s">
         <v>39</v>
       </c>
-      <c r="X10" t="s">
+      <c r="X14" t="s">
         <v>40</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Y14" t="s">
         <v>41</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="Z14" t="s">
         <v>62</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AA14" t="s">
         <v>31</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AB14" t="s">
         <v>33</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AC14" t="s">
         <v>35</v>
       </c>
-      <c r="AD10" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE10">
-        <v>1</v>
-      </c>
-      <c r="AF10">
-        <v>1</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH10" t="s">
+      <c r="AD14" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE14">
+        <v>1</v>
+      </c>
+      <c r="AF14">
+        <v>1</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B15" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D15" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J15" t="s">
         <v>21</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K15" t="s">
         <v>22</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L15" t="s">
         <v>12</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M15" t="s">
         <v>17</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N15" t="s">
         <v>18</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O15" t="s">
         <v>48</v>
       </c>
-      <c r="P11">
+      <c r="P15">
         <v>967</v>
       </c>
-      <c r="Q11" t="s">
-        <v>6</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="Q15" t="s">
+        <v>6</v>
+      </c>
+      <c r="R15" t="s">
         <v>23</v>
       </c>
-      <c r="S11">
+      <c r="S15">
         <v>25698369</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T15" t="s">
         <v>46</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U15" t="s">
         <v>47</v>
       </c>
-      <c r="V11">
+      <c r="V15">
         <v>2020</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W15" t="s">
         <v>39</v>
       </c>
-      <c r="X11" t="s">
+      <c r="X15" t="s">
         <v>40</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Y15" t="s">
         <v>41</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="Z15" t="s">
         <v>63</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AA15" t="s">
         <v>31</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AB15" t="s">
         <v>33</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AC15" t="s">
         <v>35</v>
       </c>
-      <c r="AD11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE11">
-        <v>1</v>
-      </c>
-      <c r="AF11">
-        <v>1</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH11" t="s">
+      <c r="AD15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE15">
+        <v>1</v>
+      </c>
+      <c r="AF15">
+        <v>1</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J16" t="s">
         <v>21</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K16" t="s">
         <v>22</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L16" t="s">
         <v>12</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M16" t="s">
         <v>17</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N16" t="s">
         <v>18</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O16" t="s">
         <v>49</v>
       </c>
-      <c r="P12">
+      <c r="P16">
         <v>967</v>
       </c>
-      <c r="Q12" t="s">
-        <v>6</v>
-      </c>
-      <c r="R12" t="s">
+      <c r="Q16" t="s">
+        <v>6</v>
+      </c>
+      <c r="R16" t="s">
         <v>23</v>
       </c>
-      <c r="S12">
+      <c r="S16">
         <v>25698369</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T16" t="s">
         <v>51</v>
       </c>
-      <c r="U12" t="s">
+      <c r="U16" t="s">
         <v>55</v>
       </c>
-      <c r="V12">
+      <c r="V16">
         <v>2020</v>
       </c>
-      <c r="W12" t="s">
+      <c r="W16" t="s">
         <v>39</v>
       </c>
-      <c r="X12" t="s">
+      <c r="X16" t="s">
         <v>40</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Y16" t="s">
         <v>41</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="Z16" t="s">
         <v>64</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AA16" t="s">
         <v>31</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AB16" t="s">
         <v>33</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AC16" t="s">
         <v>35</v>
       </c>
-      <c r="AD12" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE12">
-        <v>1</v>
-      </c>
-      <c r="AF12">
-        <v>1</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH12" t="s">
+      <c r="AD16" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE16">
+        <v>1</v>
+      </c>
+      <c r="AF16">
+        <v>1</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1918,17 +2334,21 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C12" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="C2" r:id="rId7" xr:uid="{9382C0EF-D38A-4EE2-B93D-495E1004483D}"/>
     <hyperlink ref="C5" r:id="rId8" xr:uid="{433A40A7-91DC-489F-83E8-361329B290F3}"/>
     <hyperlink ref="C6" r:id="rId9" xr:uid="{0790693F-CF10-4F60-9F23-490A41178744}"/>
-    <hyperlink ref="C7" r:id="rId10" xr:uid="{5D7CF031-FC68-4343-9406-07538E7BAB70}"/>
-    <hyperlink ref="C8" r:id="rId11" xr:uid="{435D7301-CBB5-466B-A334-F577EF067C76}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{5D7CF031-FC68-4343-9406-07538E7BAB70}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{435D7301-CBB5-466B-A334-F577EF067C76}"/>
+    <hyperlink ref="C9" r:id="rId12" xr:uid="{9F7B37C8-74F9-4DD8-9D48-D13B488289D5}"/>
+    <hyperlink ref="C10" r:id="rId13" xr:uid="{541F826F-E21D-4A12-A9EB-7728315E5210}"/>
+    <hyperlink ref="C7" r:id="rId14" xr:uid="{4CD87077-B036-4925-9A38-A07941A96797}"/>
+    <hyperlink ref="C8" r:id="rId15" xr:uid="{86F97C9E-7382-4A20-9EE5-ACF5D03A33BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
precondiciones y creacion de acuerdos
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotorTercero.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotorTercero.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC360C9-6274-4C4A-B79A-EA165CD3331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC74AF8-AE07-4CFB-A700-DC64057D117F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AG9" sqref="AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="8" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>45</v>
@@ -1492,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="5" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="AH8" s="5" t="s">
         <v>6</v>

</xml_diff>